<commit_message>
fix table, calculation of pot and scatt values, improve output figure
</commit_message>
<xml_diff>
--- a/transitions.xlsx
+++ b/transitions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="315">
   <si>
     <t>0.035</t>
   </si>
@@ -970,6 +970,28 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 P ⴰ1/2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1592,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K349"/>
+  <dimension ref="A1:L349"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="H174" sqref="H174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5534,9 +5556,7 @@
       <c r="E176" s="21"/>
       <c r="F176" s="21"/>
       <c r="G176" s="21"/>
-      <c r="H176" s="27">
-        <v>793800</v>
-      </c>
+      <c r="H176" s="27"/>
       <c r="I176" s="21" t="s">
         <v>1</v>
       </c>
@@ -5851,8 +5871,8 @@
         <v>2.5</v>
       </c>
       <c r="H190" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A190*10^-10)^3)*(2*F190+1)/(2*G190+1)*E190^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>4959605.5791599741</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A190*10^-10)^3)*(2*F190+1)/(2*G190+1)*E190^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>2479802.7895799871</v>
       </c>
       <c r="I190" s="15" t="s">
         <v>178</v>
@@ -5926,8 +5946,8 @@
         <v>2.5</v>
       </c>
       <c r="H193" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A193*10^-10)^3)*(2*F193+1)/(2*G193+1)*E193^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>7241782.7098240219</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A193*10^-10)^3)*(2*F193+1)/(2*G193+1)*E193^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>3620891.354912011</v>
       </c>
       <c r="I193" s="15" t="s">
         <v>178</v>
@@ -6509,8 +6529,8 @@
         <v>0.5</v>
       </c>
       <c r="H219" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A219*10^-10)^3)*(2*F219+1)/(2*G219+1)*E219^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>365025.49296997074</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A219*10^-10)^3)*(2*F219+1)/(2*G219+1)*E219^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>182512.74648498537</v>
       </c>
       <c r="I219" s="17" t="s">
         <v>132</v>
@@ -6542,8 +6562,8 @@
         <v>1.5</v>
       </c>
       <c r="H220" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A220*10^-10)^3)*(2*F220+1)/(2*G220+1)*E220^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>6349292.6684332462</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A220*10^-10)^3)*(2*F220+1)/(2*G220+1)*E220^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>3174646.3342166231</v>
       </c>
       <c r="I220" s="15" t="s">
         <v>178</v>
@@ -6575,8 +6595,8 @@
         <v>1.5</v>
       </c>
       <c r="H221" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A221*10^-10)^3)*(2*F221+1)/(2*G221+1)*E221^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>441041.56061682309</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A221*10^-10)^3)*(2*F221+1)/(2*G221+1)*E221^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>220520.78030841154</v>
       </c>
       <c r="I221" s="19" t="s">
         <v>135</v>
@@ -6696,8 +6716,8 @@
         <v>2.5</v>
       </c>
       <c r="H226" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A226*10^-10)^3)*(2*F226+1)/(2*G226+1)*E226^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>33331989.586952347</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A226*10^-10)^3)*(2*F226+1)/(2*G226+1)*E226^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>16665994.793476174</v>
       </c>
       <c r="I226" s="15" t="s">
         <v>178</v>
@@ -6727,8 +6747,8 @@
         <v>1.5</v>
       </c>
       <c r="H227" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A227*10^-10)^3)*(2*F227+1)/(2*G227+1)*E227^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>5665678.2439390849</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A227*10^-10)^3)*(2*F227+1)/(2*G227+1)*E227^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>2832839.1219695425</v>
       </c>
       <c r="I227" s="4" t="s">
         <v>178</v>
@@ -6760,8 +6780,8 @@
         <v>0.5</v>
       </c>
       <c r="H228" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A228*10^-10)^3)*(2*F228+1)/(2*G228+1)*E228^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>570340.27308121417</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A228*10^-10)^3)*(2*F228+1)/(2*G228+1)*E228^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>285170.13654060708</v>
       </c>
       <c r="I228" s="17" t="s">
         <v>132</v>
@@ -6793,8 +6813,8 @@
         <v>1.5</v>
       </c>
       <c r="H229" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A229*10^-10)^3)*(2*F229+1)/(2*G229+1)*E229^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>686146.2444751357</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A229*10^-10)^3)*(2*F229+1)/(2*G229+1)*E229^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>343073.12223756785</v>
       </c>
       <c r="I229" s="19" t="s">
         <v>135</v>
@@ -6940,8 +6960,8 @@
         <v>0.5</v>
       </c>
       <c r="H235" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A235*10^-10)^3)*(2*F235+1)/(2*G235+1)*E235^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>1075405.5178051994</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A235*10^-10)^3)*(2*F235+1)/(2*G235+1)*E235^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>537702.75890259969</v>
       </c>
       <c r="I235" s="17" t="s">
         <v>132</v>
@@ -7064,7 +7084,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="51">
         <v>8521.1316530000004</v>
       </c>
@@ -7088,7 +7108,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="52">
         <v>8761.4120999999996</v>
       </c>
@@ -7112,7 +7132,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="54">
         <v>8853.2021000000004</v>
       </c>
@@ -7138,7 +7158,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="54">
         <v>8918.4989999999998</v>
       </c>
@@ -7169,8 +7189,11 @@
       <c r="J244" s="17" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K244" s="28">
+        <v>513000</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="55">
         <v>8930.3770000000004</v>
       </c>
@@ -7201,8 +7224,11 @@
       <c r="J245" s="19" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K245" s="28">
+        <v>397000</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="51">
         <v>8943.4742387599999</v>
       </c>
@@ -7226,7 +7252,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="53">
         <v>9172.3178000000007</v>
       </c>
@@ -7248,7 +7274,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="53">
         <v>9208.5337999999992</v>
       </c>
@@ -7272,7 +7298,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="56">
         <v>9783.8309000000008</v>
       </c>
@@ -7295,8 +7321,8 @@
         <v>1.5</v>
       </c>
       <c r="H249" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A249*10^-10)^3)*(2*F249+1)/(2*G249+1)*E249^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>169591.31391807122</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A249*10^-10)^3)*(2*F249+1)/(2*G249+1)*E249^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>84795.656959035608</v>
       </c>
       <c r="I249" s="7" t="s">
         <v>227</v>
@@ -7305,7 +7331,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="56">
         <v>9809.6209999999992</v>
       </c>
@@ -7328,8 +7354,8 @@
         <v>0.5</v>
       </c>
       <c r="H250" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A250*10^-10)^3)*(2*F250+1)/(2*G250+1)*E250^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>78777.893995912222</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A250*10^-10)^3)*(2*F250+1)/(2*G250+1)*E250^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>39388.946997956111</v>
       </c>
       <c r="I250" s="7" t="s">
         <v>227</v>
@@ -7338,7 +7364,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="57" t="s">
         <v>228</v>
       </c>
@@ -7352,7 +7378,7 @@
       <c r="I251" s="2"/>
       <c r="J251" s="2"/>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="54">
         <v>10027.103300000001</v>
       </c>
@@ -7376,7 +7402,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="55">
         <v>10126.188</v>
       </c>
@@ -7400,7 +7426,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="55">
         <v>10126.376700000001</v>
       </c>
@@ -7424,7 +7450,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="56">
         <v>10933.567999999999</v>
       </c>
@@ -7447,8 +7473,8 @@
         <v>1.5</v>
       </c>
       <c r="H255" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A255*10^-10)^3)*(2*F255+1)/(2*G255+1)*E255^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>358468.45987095137</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A255*10^-10)^3)*(2*F255+1)/(2*G255+1)*E255^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>179234.22993547568</v>
       </c>
       <c r="I255" s="7" t="s">
         <v>227</v>
@@ -7457,7 +7483,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="56">
         <v>10987.243</v>
       </c>
@@ -7480,11 +7506,11 @@
         <v>0.5</v>
       </c>
       <c r="H256" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A256*10^-10)^3)*(2*F256+1)/(2*G256+1)*E256^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>186124.50293375165</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A256*10^-10)^3)*(2*F256+1)/(2*G256+1)*E256^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>93062.251466875823</v>
       </c>
       <c r="I256" s="7" t="s">
-        <v>227</v>
+        <v>313</v>
       </c>
       <c r="J256" s="7" t="s">
         <v>158</v>
@@ -7882,7 +7908,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" s="50">
         <v>13575.189</v>
       </c>
@@ -7906,7 +7932,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" s="52">
         <v>13592.008</v>
       </c>
@@ -7928,8 +7954,9 @@
       <c r="G274" s="13">
         <v>0.5</v>
       </c>
-      <c r="H274" s="27">
-        <v>6230000</v>
+      <c r="H274" s="5">
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A274*10^-10)^3)*(2*F274+1)/(2*G274+1)*E274^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>7254804.726735875</v>
       </c>
       <c r="I274" s="13" t="s">
         <v>172</v>
@@ -7938,8 +7965,11 @@
         <v>227</v>
       </c>
       <c r="K274" s="45"/>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L274" s="27">
+        <v>6230000</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" s="60">
         <v>13606.276</v>
       </c>
@@ -7965,8 +7995,11 @@
         <v>170</v>
       </c>
       <c r="K275" s="45"/>
-    </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L275" s="32">
+        <v>1590000</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" s="54">
         <v>13762.57</v>
       </c>
@@ -7998,8 +8031,11 @@
         <v>171</v>
       </c>
       <c r="K276" s="45"/>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L276" s="32">
+        <v>1590000</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" s="56">
         <v>13781.739</v>
       </c>
@@ -8031,8 +8067,11 @@
         <v>161</v>
       </c>
       <c r="K277" s="45"/>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L277" s="28">
+        <v>565000</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" s="59">
         <v>13917.2397</v>
       </c>
@@ -8057,7 +8096,7 @@
       </c>
       <c r="K278" s="45"/>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" s="56">
         <v>13940.5767</v>
       </c>
@@ -8080,20 +8119,20 @@
         <v>0.5</v>
       </c>
       <c r="H279" s="5">
-        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A279*10^-10)^3)*(2*F279+1)/(2*G279+1)*E279^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2</f>
-        <v>13448206.424299587</v>
+        <f>(8*(3.14159)^2)/(3*8.85419*10^-12*1.0545718*10^-34*(A279*10^-10)^3)*(2*F279+1)/(2*G279+1)*E279^2*(5.2917721092*10^-11)^2 * (1.602*10^-19)^2 * 1/2</f>
+        <v>6724103.2121497933</v>
       </c>
       <c r="I279" s="7" t="s">
         <v>227</v>
       </c>
       <c r="J279" s="7" t="s">
-        <v>172</v>
+        <v>314</v>
       </c>
       <c r="K279" s="47" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" s="50">
         <v>14104.531999999999</v>
       </c>
@@ -8118,7 +8157,7 @@
       </c>
       <c r="K280" s="45"/>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" s="50">
         <v>14157.616</v>
       </c>
@@ -8143,7 +8182,7 @@
       </c>
       <c r="K281" s="45"/>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" s="50">
         <v>14190.434999999999</v>
       </c>
@@ -8168,7 +8207,7 @@
       </c>
       <c r="K282" s="45"/>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" s="59">
         <v>14515.050999999999</v>
       </c>
@@ -8193,7 +8232,7 @@
       </c>
       <c r="K283" s="45"/>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" s="59">
         <v>14530.052</v>
       </c>
@@ -8218,7 +8257,7 @@
       </c>
       <c r="K284" s="45"/>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" s="50">
         <v>14674.373</v>
       </c>
@@ -8243,7 +8282,7 @@
       </c>
       <c r="K285" s="45"/>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286" s="53">
         <v>14698.924999999999</v>
       </c>
@@ -8276,7 +8315,7 @@
       </c>
       <c r="K286" s="45"/>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287" s="50">
         <v>14729.413</v>
       </c>
@@ -8300,7 +8339,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288" s="50">
         <v>15245.859</v>
       </c>

</xml_diff>